<commit_message>
set up fetch to google
</commit_message>
<xml_diff>
--- a/src/parcer-excel.xlsx
+++ b/src/parcer-excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex.n\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sublimegit\kottans\framework-2021-weather-app\framework-2021\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>START DATE</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t>Chemistry</t>
+  </si>
+  <si>
+    <t>03/24/2019</t>
+  </si>
+  <si>
+    <t>03/24/2020</t>
+  </si>
+  <si>
+    <t>03/24/2021</t>
+  </si>
+  <si>
+    <t>03/24/2022</t>
+  </si>
+  <si>
+    <t>03/24/2023</t>
   </si>
 </sst>
 </file>
@@ -69,12 +84,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -83,7 +113,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -366,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,6 +437,90 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
preparation for download from remote
</commit_message>
<xml_diff>
--- a/src/parcer-excel.xlsx
+++ b/src/parcer-excel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex.n\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kottans\weather-app\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23232" windowHeight="10824"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23235" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>START DATE</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Chemistry</t>
+  </si>
+  <si>
+    <t>03/24/2019</t>
+  </si>
+  <si>
+    <t>03/24/2020</t>
+  </si>
+  <si>
+    <t>03/24/2021</t>
   </si>
 </sst>
 </file>
@@ -366,20 +375,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -393,7 +402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -404,6 +413,48 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>